<commit_message>
update new instructions 2 and 7
</commit_message>
<xml_diff>
--- a/new_instructions_2.xlsx
+++ b/new_instructions_2.xlsx
@@ -20,10 +20,10 @@
     <t xml:space="preserve">Before each story, you will be assigned one of the eight perspectives to take on while reading it. </t>
   </si>
   <si>
-    <t xml:space="preserve">You'll be given a quiz before the story for the 4 questions of the assigned perspective. </t>
+    <t xml:space="preserve">You'll be given a quiz before the story for the 4 questions associated with the assigned perspective. </t>
   </si>
   <si>
-    <t xml:space="preserve">You must pass this quiz to move onto the story, but you will have a few chances. </t>
+    <t xml:space="preserve">You must pass this quiz to move onto the story. </t>
   </si>
 </sst>
 </file>
@@ -1457,7 +1457,7 @@
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
     </row>
-    <row r="3" ht="94.55" customHeight="1">
+    <row r="3" ht="109.55" customHeight="1">
       <c r="A3" t="s" s="4">
         <v>2</v>
       </c>
@@ -1468,7 +1468,7 @@
       <c r="F3" s="8"/>
       <c r="G3" s="8"/>
     </row>
-    <row r="4" ht="94.55" customHeight="1">
+    <row r="4" ht="64.55" customHeight="1">
       <c r="A4" t="s" s="4">
         <v>3</v>
       </c>

</xml_diff>